<commit_message>
Updated solver file and example datasets
</commit_message>
<xml_diff>
--- a/vignettes/Example_uncertain_variables.xlsx
+++ b/vignettes/Example_uncertain_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Documents\GitHub\SimpleBox\SBooScripts\vignettes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ABCC8B-BA42-4FCF-A0A9-65016C98A4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C4A6F3-667F-4203-90BA-D7099BAE1D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Update notes</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>varName</t>
+  </si>
+  <si>
+    <t>RadS</t>
   </si>
 </sst>
 </file>
@@ -258,10 +261,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,7 +643,9 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -713,6 +714,23 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>2500000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
     </row>
@@ -738,21 +756,18 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D49:D50" xr:uid="{6C20B6BE-CD2E-4471-81F1-E8281B3E4F14}">
       <formula1>"Triangular,Uniform,Powerlaw"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D48" xr:uid="{63A27DCE-AD25-4102-9035-0521D66C4A62}">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{63A27DCE-AD25-4102-9035-0521D66C4A62}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D48</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD7D180D-0C3B-40D2-824E-2D06F6EBC901}">
           <x14:formula1>
             <xm:f>Distributions!$A$2:$A$15</xm:f>
@@ -773,7 +788,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,28 +874,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF634CA3F5682C418397C6E4414BCDE3" ma:contentTypeVersion="19" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="cd864e38cd6bbc6c7e0427721adcc1d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0577e6a0-5f74-4659-a81a-c7bdc984432d" xmlns:ns3="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa37df3857ed3652683061e5b337c961" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1146,10 +1139,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB164739-7153-45E5-8FBB-FF9181C40EB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE058C2-4EA7-449D-8837-75A59343C78C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
+    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1173,21 +1200,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE058C2-4EA7-449D-8837-75A59343C78C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB164739-7153-45E5-8FBB-FF9181C40EB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
-    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>